<commit_message>
improve codes and add more testing for file api
</commit_message>
<xml_diff>
--- a/maple_api/media/file/files/test.xlsx
+++ b/maple_api/media/file/files/test.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="37">
   <si>
     <t>id</t>
   </si>
@@ -76,12 +76,18 @@
     <t>paypal_order_id</t>
   </si>
   <si>
+    <t>1</t>
+  </si>
+  <si>
     <t>default</t>
   </si>
   <si>
     <t>USD</t>
   </si>
   <si>
+    <t>1.77</t>
+  </si>
+  <si>
     <t>gold</t>
   </si>
   <si>
@@ -103,6 +109,9 @@
     <t>San Jose</t>
   </si>
   <si>
+    <t>95131</t>
+  </si>
+  <si>
     <t>US</t>
   </si>
   <si>
@@ -113,22 +122,17 @@
   </si>
   <si>
     <t>ELIGIBLE</t>
+  </si>
+  <si>
+    <t>s</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -144,7 +148,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -152,30 +156,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -470,134 +456,146 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T2"/>
+  <dimension ref="A1:X2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:20">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:24">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="S1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="T1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:20">
-      <c r="A2">
-        <v>1</v>
+    <row r="2" spans="1:24">
+      <c r="A2" t="s">
+        <v>20</v>
       </c>
       <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K2" t="s">
+        <v>30</v>
+      </c>
+      <c r="L2" t="s">
+        <v>31</v>
+      </c>
+      <c r="M2" t="s">
+        <v>32</v>
+      </c>
+      <c r="N2" t="s">
+        <v>33</v>
+      </c>
+      <c r="O2" t="s">
+        <v>34</v>
+      </c>
+      <c r="P2" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>23</v>
+      </c>
+      <c r="R2" t="s">
         <v>20</v>
       </c>
-      <c r="C2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2">
-        <v>1.77</v>
-      </c>
-      <c r="E2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G2" t="s">
-        <v>24</v>
-      </c>
-      <c r="H2" t="s">
-        <v>25</v>
-      </c>
-      <c r="I2" t="s">
-        <v>26</v>
-      </c>
-      <c r="J2" t="s">
-        <v>27</v>
-      </c>
-      <c r="K2" t="s">
-        <v>28</v>
-      </c>
-      <c r="L2">
-        <v>95131</v>
-      </c>
-      <c r="M2" t="s">
-        <v>29</v>
-      </c>
-      <c r="N2" t="s">
-        <v>30</v>
-      </c>
-      <c r="O2" t="s">
-        <v>31</v>
-      </c>
-      <c r="P2" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q2">
-        <v>1.77</v>
-      </c>
-      <c r="R2">
-        <v>1</v>
-      </c>
       <c r="S2" t="s">
-        <v>32</v>
-      </c>
-      <c r="T2">
-        <v>1</v>
+        <v>35</v>
+      </c>
+      <c r="T2" t="s">
+        <v>20</v>
+      </c>
+      <c r="U2" t="s">
+        <v>36</v>
+      </c>
+      <c r="V2" t="s">
+        <v>36</v>
+      </c>
+      <c r="W2" t="s">
+        <v>36</v>
+      </c>
+      <c r="X2" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>